<commit_message>
Fixing a set for departement and position in xlsxReader
</commit_message>
<xml_diff>
--- a/src/main/resources/filedatestare/excelFile.xlsx
+++ b/src/main/resources/filedatestare/excelFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.vergine\Desktop\filedatestare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\corso_its\projects\Fincons-Employees-BE\src\main\resources\filedatestare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9177ADB5-5153-4512-8129-0612D43AC4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA178E3F-EC0E-409F-AB7B-011BCDEF98BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27192" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{1B7CC18F-ED34-407C-8F65-7EC2BE0F0B8A}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B7CC18F-ED34-407C-8F65-7EC2BE0F0B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF4DD18C-F0FD-4DD9-9DCB-0471B8CD6734}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,6 +627,8 @@
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -681,10 +683,10 @@
         <v>46022</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -710,10 +712,10 @@
         <v>45580</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -739,10 +741,10 @@
         <v>46295</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -768,10 +770,10 @@
         <v>46446</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -800,7 +802,7 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -826,10 +828,10 @@
         <v>46127</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -855,10 +857,10 @@
         <v>45534</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -884,10 +886,10 @@
         <v>45981</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -913,10 +915,10 @@
         <v>46188</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -942,10 +944,10 @@
         <v>45940</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -971,10 +973,10 @@
         <v>46106</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1000,10 +1002,10 @@
         <v>46392</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1032,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1058,10 +1060,10 @@
         <v>46223</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1087,10 +1089,10 @@
         <v>46487</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1116,7 +1118,7 @@
         <v>45792</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -1145,10 +1147,10 @@
         <v>45626</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1174,7 +1176,7 @@
         <v>46466</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1194,7 +1196,7 @@
         <v>44887</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F20" s="1">
         <v>44689</v>
@@ -1203,10 +1205,10 @@
         <v>45894</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1222,8 +1224,8 @@
       <c r="D21" s="1">
         <v>44888</v>
       </c>
-      <c r="E21" t="s">
-        <v>67</v>
+      <c r="E21" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="F21" s="1">
         <v>44690</v>
@@ -1232,17 +1234,18 @@
         <v>45895</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E20" r:id="rId1" xr:uid="{E91A2D51-CCBA-42CA-AAC2-29C5DB642431}"/>
+    <hyperlink ref="E21" r:id="rId2" xr:uid="{324B5C85-46E3-4FAF-8CB1-62D07227434B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiunta di altri file per testare api di Import File
</commit_message>
<xml_diff>
--- a/src/main/resources/filedatestare/excelFile.xlsx
+++ b/src/main/resources/filedatestare/excelFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\corso_its\projects\Fincons-Employees-BE\src\main\resources\filedatestare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA178E3F-EC0E-409F-AB7B-011BCDEF98BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56970172-B4E2-4B7A-AB06-9A618932BA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B7CC18F-ED34-407C-8F65-7EC2BE0F0B8A}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>giovanni@moretti.it</t>
-  </si>
-  <si>
     <t>Laura</t>
   </si>
   <si>
@@ -86,169 +83,172 @@
     <t>F</t>
   </si>
   <si>
-    <t>laura@ricci.it</t>
-  </si>
-  <si>
     <t>Alessandro</t>
   </si>
   <si>
     <t>Galli</t>
   </si>
   <si>
-    <t>alessandro@galli.it</t>
-  </si>
-  <si>
     <t>Simona</t>
   </si>
   <si>
     <t>Bianco</t>
   </si>
   <si>
-    <t>simona@bianco.it</t>
-  </si>
-  <si>
     <t>Daniele</t>
   </si>
   <si>
     <t>Ferrari</t>
   </si>
   <si>
-    <t>daniele@ferrari.it</t>
-  </si>
-  <si>
     <t>Elena</t>
   </si>
   <si>
     <t>Rossini</t>
   </si>
   <si>
-    <t>elena@rossini.it</t>
-  </si>
-  <si>
     <t>Roberto</t>
   </si>
   <si>
     <t>Greco</t>
   </si>
   <si>
-    <t>roberto@greco.it</t>
-  </si>
-  <si>
     <t>Silvia</t>
   </si>
   <si>
     <t>Conti</t>
   </si>
   <si>
-    <t>silvia@conti.it</t>
-  </si>
-  <si>
     <t>Marco</t>
   </si>
   <si>
     <t>Marini</t>
   </si>
   <si>
-    <t>marco@marini.it</t>
-  </si>
-  <si>
     <t>Valentina</t>
   </si>
   <si>
     <t>Santoro</t>
   </si>
   <si>
-    <t>valentina@santoro.it</t>
-  </si>
-  <si>
     <t>Nicola</t>
   </si>
   <si>
     <t>Gallo</t>
   </si>
   <si>
-    <t>nicola@gallo.it</t>
-  </si>
-  <si>
     <t>Giorgia</t>
   </si>
   <si>
     <t>Barbieri</t>
   </si>
   <si>
-    <t>giorgia@barbieri.it</t>
-  </si>
-  <si>
     <t>Luigi</t>
   </si>
   <si>
     <t>Fontana</t>
   </si>
   <si>
-    <t>luigi@fontana.it</t>
-  </si>
-  <si>
     <t>Elisa</t>
   </si>
   <si>
     <t>Morelli</t>
   </si>
   <si>
-    <t>elisa@morelli.it</t>
-  </si>
-  <si>
     <t>Francesco</t>
   </si>
   <si>
     <t>Riva</t>
   </si>
   <si>
-    <t>francesco@riva.it</t>
-  </si>
-  <si>
     <t>Martina</t>
   </si>
   <si>
     <t>Lombardi</t>
   </si>
   <si>
-    <t>martina@lombardi.it</t>
-  </si>
-  <si>
     <t>Paolo</t>
   </si>
   <si>
     <t>Colombo</t>
   </si>
   <si>
-    <t>paolo@colombo.it</t>
-  </si>
-  <si>
     <t>Federica</t>
   </si>
   <si>
     <t>Caruso</t>
   </si>
   <si>
-    <t>federica@caruso.it</t>
-  </si>
-  <si>
     <t>Riccardo</t>
   </si>
   <si>
     <t>Gatti</t>
   </si>
   <si>
-    <t>riccardo@gatti.it</t>
-  </si>
-  <si>
-    <t>riccardo@gattinone.it</t>
-  </si>
-  <si>
     <t>Riccardino</t>
   </si>
   <si>
     <t>Gattinone</t>
+  </si>
+  <si>
+    <t>giovanni@gmail.com</t>
+  </si>
+  <si>
+    <t>laura@gmail.com</t>
+  </si>
+  <si>
+    <t>alessandro@gmail.com</t>
+  </si>
+  <si>
+    <t>simona@gmail.com</t>
+  </si>
+  <si>
+    <t>daniele@gmail.com</t>
+  </si>
+  <si>
+    <t>elena@gmail.com</t>
+  </si>
+  <si>
+    <t>roberto@gmail.com</t>
+  </si>
+  <si>
+    <t>silvia@gmail.com</t>
+  </si>
+  <si>
+    <t>marco@gmail.com</t>
+  </si>
+  <si>
+    <t>valentina@gmail.com</t>
+  </si>
+  <si>
+    <t>nicola@gmail.com</t>
+  </si>
+  <si>
+    <t>giorgia@gmail.com</t>
+  </si>
+  <si>
+    <t>elisa@gmail.com</t>
+  </si>
+  <si>
+    <t>francesco@gmail.com</t>
+  </si>
+  <si>
+    <t>martina@gmail.com</t>
+  </si>
+  <si>
+    <t>paolo@gmail.com</t>
+  </si>
+  <si>
+    <t>riccardo@gmail.com</t>
+  </si>
+  <si>
+    <t>riccardino@gmail.com</t>
+  </si>
+  <si>
+    <t>luigi@gmail.com</t>
+  </si>
+  <si>
+    <t>federica@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -618,7 +618,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,7 +674,7 @@
         <v>45000</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="F2" s="1">
         <v>44814</v>
@@ -691,19 +691,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
       </c>
       <c r="D3" s="1">
         <v>44794</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="F3" s="1">
         <v>44531</v>
@@ -720,10 +720,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -732,7 +732,7 @@
         <v>45265</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1">
         <v>45066</v>
@@ -749,19 +749,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1">
         <v>45430</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="F5" s="1">
         <v>45260</v>
@@ -778,10 +778,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -790,7 +790,7 @@
         <v>44864</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="F6" s="1">
         <v>44666</v>
@@ -807,19 +807,19 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1">
         <v>45324</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="F7" s="1">
         <v>45160</v>
@@ -836,10 +836,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -848,7 +848,7 @@
         <v>44724</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="F8" s="1">
         <v>44525</v>
@@ -865,19 +865,19 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1">
         <v>45023</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="F9" s="1">
         <v>44849</v>
@@ -894,10 +894,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -906,7 +906,7 @@
         <v>45545</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1">
         <v>45021</v>
@@ -923,19 +923,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1">
         <v>44910</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F11" s="1">
         <v>44711</v>
@@ -952,10 +952,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -964,7 +964,7 @@
         <v>45127</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="F12" s="1">
         <v>44936</v>
@@ -981,19 +981,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1">
         <v>45299</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="F13" s="1">
         <v>45125</v>
@@ -1010,10 +1010,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1021,8 +1021,8 @@
       <c r="D14" s="1">
         <v>44676</v>
       </c>
-      <c r="E14" t="s">
-        <v>49</v>
+      <c r="E14" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F14" s="1">
         <v>44479</v>
@@ -1039,19 +1039,19 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1">
         <v>45199</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="F15" s="1">
         <v>45000</v>
@@ -1068,10 +1068,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -1080,7 +1080,7 @@
         <v>45363</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F16" s="1">
         <v>45170</v>
@@ -1097,19 +1097,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1">
         <v>44747</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F17" s="1">
         <v>44550</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1138,7 +1138,7 @@
         <v>44946</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F18" s="1">
         <v>44714</v>
@@ -1155,19 +1155,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1">
         <v>45471</v>
       </c>
-      <c r="E19" t="s">
-        <v>64</v>
+      <c r="E19" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F19" s="1">
         <v>44941</v>
@@ -1184,10 +1184,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -1213,10 +1213,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -1242,10 +1242,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E20" r:id="rId1" xr:uid="{E91A2D51-CCBA-42CA-AAC2-29C5DB642431}"/>
-    <hyperlink ref="E21" r:id="rId2" xr:uid="{324B5C85-46E3-4FAF-8CB1-62D07227434B}"/>
+    <hyperlink ref="E21" r:id="rId1" xr:uid="{324B5C85-46E3-4FAF-8CB1-62D07227434B}"/>
+    <hyperlink ref="E14" r:id="rId2" xr:uid="{1DFFAC72-7D17-4069-BA6B-8BA36A3AAFF2}"/>
+    <hyperlink ref="E19" r:id="rId3" xr:uid="{DB4DCC4D-239B-4DF3-8B74-30BA704A8D22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>